<commit_message>
Places to avoid added
</commit_message>
<xml_diff>
--- a/RECORD.xlsx
+++ b/RECORD.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jay\Desktop\tourist2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D63B591C-62C2-4B10-871D-995266EF511D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9A3B10E-D7AC-43A0-A78B-0A127A57E3D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2205" yWindow="2205" windowWidth="15375" windowHeight="7890" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="81">
   <si>
     <t>MUMBAI</t>
   </si>
@@ -279,12 +279,50 @@
   <si>
     <t>https://img.traveltriangle.com/blog/wp-content/uploads/2018/03/82-e1576479223141.jpg</t>
   </si>
+  <si>
+    <t xml:space="preserve">1.Taxi or the Mumbai Auto drivers may charge you more as you won't have idea about the fare so rather go for services like ola uber.
+2.Young Beggar Girl with the baby asking for Milk or Money.
+3.Old lady asking for food and you fail to avoid she may run behind you so you have to be harsh.
+4.Local stores may cheat you by selling goods at higher rates if they find you aren't local. </t>
+  </si>
+  <si>
+    <t>JAIPUR</t>
+  </si>
+  <si>
+    <t>Jaipur is a vibrant amalgamation of the old and the new. Also called the Pink City, the capital of the royal state of Rajasthan, was ruled by the Rajputs for many centuries and developed as a planned city in the 17th century AD. Along with Delhi and Agra, Jaipur forms the Golden Triangle and hails as one of the most famous tourist circuits of the country.</t>
+  </si>
+  <si>
+    <t>AMER FORT,JAIGARH FORT,NAHARGARH FORT,HAWA MAHAL,CITY PALACE,JANTAR MANTAR,GALTAJI TEMPLE,BIRLA TEMPLE,CHOKI DHANI,PINK CITY,ALBERT HALL MUESEUM,JAL MAHAL,WORLD TRADE PARK,CHAND BOWRI.</t>
+  </si>
+  <si>
+    <t>https://encrypted-tbn0.gstatic.com/images?q=tbn%3AANd9GcQJUnPpisyM5AcjWzr_3ZLjrSo9lPpFRbDFR7MzIFfQgmGLpKA-&amp;usqp=CAU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.Young Beggar Girl with the baby asking for Milk or Money.
+2.Old lady asking for food and you fail to avoid she may run behind you so you have to be harsh.
+3.Local stores may cheat you by selling goods at higher rates if they find you aren't local.
+4.Fake Sadhu's near holy temples may promise you to tell your future in return of money. </t>
+  </si>
+  <si>
+    <t>Young Beggar Girl with the baby asking for Milk or Money,
+Old lady asking for food and you fail to avoid she may run behind you so you have to be harsh,
+Local stores may cheat you by selling goods at higher rates if they find you aren't local</t>
+  </si>
+  <si>
+    <t>Local stores may cheat you by selling goods at higher rates if they find you aren't local.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Taxi or the Mumbai Auto drivers may charge you more as you won't have idea about the fare so rather go for services like ola uber,
+Young Beggar Girl with the baby asking for Milk or Money,
+Old lady asking for food and you fail to avoid she may run behind you so you have to be harsh,
+Local stores may cheat you by selling goods at higher rates if they find you aren't local. </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -339,6 +377,30 @@
       <color rgb="FF222222"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF212529"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -357,10 +419,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -381,8 +444,22 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -596,23 +673,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D1000"/>
+  <dimension ref="A1:E1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="D1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.125" customWidth="1"/>
-    <col min="2" max="2" width="223.75" customWidth="1"/>
+    <col min="1" max="1" width="11.75" customWidth="1"/>
+    <col min="2" max="2" width="101.25" customWidth="1"/>
     <col min="3" max="3" width="85.625" customWidth="1"/>
     <col min="4" max="4" width="78.375" customWidth="1"/>
-    <col min="5" max="26" width="7.625" customWidth="1"/>
+    <col min="5" max="5" width="60.625" customWidth="1"/>
+    <col min="6" max="26" width="7.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="138" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -625,8 +703,11 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="13" t="s">
+        <v>80</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -639,8 +720,11 @@
       <c r="D2" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="E2" s="10" t="s">
+        <v>79</v>
+      </c>
     </row>
-    <row r="3" spans="1:4" ht="123.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="123.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
@@ -654,7 +738,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
@@ -668,7 +752,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="72" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="72" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>16</v>
       </c>
@@ -682,7 +766,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="75.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="75.75" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>19</v>
       </c>
@@ -696,7 +780,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="90.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="90.75" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>23</v>
       </c>
@@ -710,7 +794,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="30.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="30.75" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>27</v>
       </c>
@@ -724,7 +808,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="60.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="60.75" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>31</v>
       </c>
@@ -738,7 +822,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="75.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="75.75" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>35</v>
       </c>
@@ -752,7 +836,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="60.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="60.75" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>39</v>
       </c>
@@ -766,7 +850,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="60.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="60.75" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>43</v>
       </c>
@@ -780,7 +864,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="75.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="75.75" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>47</v>
       </c>
@@ -794,7 +878,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="60.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="100.5" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>51</v>
       </c>
@@ -807,8 +891,11 @@
       <c r="D14" s="6" t="s">
         <v>54</v>
       </c>
+      <c r="E14" s="13" t="s">
+        <v>77</v>
+      </c>
     </row>
-    <row r="15" spans="1:4" ht="75.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" ht="100.5" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
         <v>55</v>
       </c>
@@ -821,8 +908,11 @@
       <c r="D15" s="6" t="s">
         <v>58</v>
       </c>
+      <c r="E15" s="13" t="s">
+        <v>77</v>
+      </c>
     </row>
-    <row r="16" spans="1:4" ht="30.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" ht="30.75" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>59</v>
       </c>
@@ -836,7 +926,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="60.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" ht="60.75" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>63</v>
       </c>
@@ -850,7 +940,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="45.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" ht="45.75" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>67</v>
       </c>
@@ -864,18 +954,35 @@
         <v>70</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="22" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="23" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="24" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="25" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="26" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="27" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="28" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="29" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="30" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="31" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="32" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="19" spans="1:5" ht="82.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="B19" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="D19" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="E19" s="13" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="22" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="23" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="24" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="25" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="26" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="27" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="28" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="29" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="30" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="33" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="34" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="35" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1849,23 +1956,24 @@
     <hyperlink ref="B1" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
     <hyperlink ref="B2" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
     <hyperlink ref="B3" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="B6" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="B7" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="B8" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="B9" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="B10" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="B11" r:id="rId9" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="B12" r:id="rId10" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="B13" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="B14" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="B15" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="B16" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="B17" r:id="rId15" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="B18" r:id="rId16" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="B4" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="B6" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="B7" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="B8" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="B9" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="B10" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="B11" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="B12" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="B13" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="B14" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="B15" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="B16" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="B17" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="B18" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="B4" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="B19" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="portrait"/>
-  <legacyDrawing r:id="rId18"/>
+  <pageSetup orientation="portrait" r:id="rId19"/>
+  <legacyDrawing r:id="rId20"/>
 </worksheet>
 </file>
</xml_diff>